<commit_message>
add parts tab to spreadsheet
</commit_message>
<xml_diff>
--- a/spacenet/tests/quick_start/quick_start_1.xlsx
+++ b/spacenet/tests/quick_start/quick_start_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pgrogan\Documents\github\spacenet-cloud\spacenet\tests\quick_start\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C07D149-6972-44F2-9AC5-5A4717C42611}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7158F9F-3CCC-4810-BED1-0C9A0D3C7C6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-48630" yWindow="11340" windowWidth="30435" windowHeight="20445" activeTab="6" xr2:uid="{CA4D0872-40A5-4645-A72D-176383645A1C}"/>
+    <workbookView xWindow="-54690" yWindow="2595" windowWidth="25875" windowHeight="22605" activeTab="6" xr2:uid="{CA4D0872-40A5-4645-A72D-176383645A1C}"/>
   </bookViews>
   <sheets>
     <sheet name="nodes" sheetId="1" r:id="rId1"/>
@@ -19,8 +19,9 @@
     <sheet name="resources" sheetId="4" r:id="rId4"/>
     <sheet name="elements" sheetId="5" r:id="rId5"/>
     <sheet name="states" sheetId="6" r:id="rId6"/>
-    <sheet name="demand_models" sheetId="7" r:id="rId7"/>
-    <sheet name="demands" sheetId="8" r:id="rId8"/>
+    <sheet name="parts" sheetId="9" r:id="rId7"/>
+    <sheet name="demand_models" sheetId="7" r:id="rId8"/>
+    <sheet name="demands" sheetId="8" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="114">
   <si>
     <t>id</t>
   </si>
@@ -369,6 +370,21 @@
   </si>
   <si>
     <t>parts_list_enabled_list</t>
+  </si>
+  <si>
+    <t>quantity</t>
+  </si>
+  <si>
+    <t>duty_cycle</t>
+  </si>
+  <si>
+    <t>mean_time_to_failure</t>
+  </si>
+  <si>
+    <t>mean_repair_time</t>
+  </si>
+  <si>
+    <t>mass_to_repair</t>
   </si>
 </sst>
 </file>
@@ -1485,7 +1501,7 @@
   <dimension ref="A1:R14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2201,10 +2217,61 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C087CDB6-6E95-4070-A0DF-1ACAA4A5B0C0}">
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F1" t="s">
+        <v>111</v>
+      </c>
+      <c r="G1" t="s">
+        <v>112</v>
+      </c>
+      <c r="H1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F33A89FF-62A8-4D27-9DD4-AC6A11DA614F}">
   <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
@@ -2247,7 +2314,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DA0B9F5-EAB2-45BD-9D78-117278B89EA3}">
   <dimension ref="A1:D1"/>
   <sheetViews>

</xml_diff>

<commit_message>
update db_loader to handle demand models and states; update quick start 1 and 2 files
</commit_message>
<xml_diff>
--- a/spacenet/tests/quick_start/quick_start_1.xlsx
+++ b/spacenet/tests/quick_start/quick_start_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pgrogan\Documents\github\spacenet-cloud\spacenet\tests\quick_start\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7158F9F-3CCC-4810-BED1-0C9A0D3C7C6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0223BDE7-A624-4711-91CA-B8403DB7648B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-54690" yWindow="2595" windowWidth="25875" windowHeight="22605" activeTab="6" xr2:uid="{CA4D0872-40A5-4645-A72D-176383645A1C}"/>
+    <workbookView xWindow="21180" yWindow="5490" windowWidth="25875" windowHeight="22605" activeTab="4" xr2:uid="{CA4D0872-40A5-4645-A72D-176383645A1C}"/>
   </bookViews>
   <sheets>
     <sheet name="nodes" sheetId="1" r:id="rId1"/>
@@ -381,10 +381,10 @@
     <t>mean_time_to_failure</t>
   </si>
   <si>
-    <t>mean_repair_time</t>
-  </si>
-  <si>
     <t>mass_to_repair</t>
+  </si>
+  <si>
+    <t>mean_time_to_repair</t>
   </si>
 </sst>
 </file>
@@ -1500,8 +1500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2582678-5ACC-41B7-9672-3475D0373149}">
   <dimension ref="A1:R14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2098,9 +2098,6 @@
       <c r="H12">
         <v>0</v>
       </c>
-      <c r="I12">
-        <v>0</v>
-      </c>
       <c r="M12">
         <v>0.66</v>
       </c>
@@ -2133,9 +2130,6 @@
       <c r="H13">
         <v>0</v>
       </c>
-      <c r="I13">
-        <v>0</v>
-      </c>
       <c r="R13" t="s">
         <v>93</v>
       </c>
@@ -2163,9 +2157,6 @@
         <v>100</v>
       </c>
       <c r="H14">
-        <v>0</v>
-      </c>
-      <c r="I14">
         <v>0</v>
       </c>
       <c r="R14" t="s">
@@ -2220,8 +2211,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C087CDB6-6E95-4070-A0DF-1ACAA4A5B0C0}">
   <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2232,7 +2223,7 @@
     <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2256,10 +2247,10 @@
         <v>111</v>
       </c>
       <c r="G1" t="s">
+        <v>113</v>
+      </c>
+      <c r="H1" t="s">
         <v>112</v>
-      </c>
-      <c r="H1" t="s">
-        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add columns for demand rates
</commit_message>
<xml_diff>
--- a/spacenet/tests/quick_start/quick_start_1.xlsx
+++ b/spacenet/tests/quick_start/quick_start_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pgrogan\Documents\github\spacenet-cloud\spacenet\tests\quick_start\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0223BDE7-A624-4711-91CA-B8403DB7648B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BCF7814-A790-4BE1-97F4-2FDDD39A5F23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21180" yWindow="5490" windowWidth="25875" windowHeight="22605" activeTab="4" xr2:uid="{CA4D0872-40A5-4645-A72D-176383645A1C}"/>
+    <workbookView xWindow="21180" yWindow="5490" windowWidth="25875" windowHeight="22605" activeTab="8" xr2:uid="{CA4D0872-40A5-4645-A72D-176383645A1C}"/>
   </bookViews>
   <sheets>
     <sheet name="nodes" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="115">
   <si>
     <t>id</t>
   </si>
@@ -385,6 +385,9 @@
   </si>
   <si>
     <t>mean_time_to_repair</t>
+  </si>
+  <si>
+    <t>rate</t>
   </si>
 </sst>
 </file>
@@ -1500,7 +1503,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2582678-5ACC-41B7-9672-3475D0373149}">
   <dimension ref="A1:R14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
@@ -2307,10 +2310,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DA0B9F5-EAB2-45BD-9D78-117278B89EA3}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="T14" sqref="T14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2321,7 +2324,7 @@
     <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2333,6 +2336,9 @@
       </c>
       <c r="D1" t="s">
         <v>104</v>
+      </c>
+      <c r="E1" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add `contents` tab to database spreadsheet to store contents of resource containers
</commit_message>
<xml_diff>
--- a/spacenet/tests/quick_start/quick_start_1.xlsx
+++ b/spacenet/tests/quick_start/quick_start_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pgrogan\Documents\github\spacenet-cloud\spacenet\tests\quick_start\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BCF7814-A790-4BE1-97F4-2FDDD39A5F23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1BF8CCC-C6C0-43A2-AEDD-58053DECBE41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21180" yWindow="5490" windowWidth="25875" windowHeight="22605" activeTab="8" xr2:uid="{CA4D0872-40A5-4645-A72D-176383645A1C}"/>
+    <workbookView xWindow="18555" yWindow="3975" windowWidth="32970" windowHeight="25995" activeTab="7" xr2:uid="{CA4D0872-40A5-4645-A72D-176383645A1C}"/>
   </bookViews>
   <sheets>
     <sheet name="nodes" sheetId="1" r:id="rId1"/>
@@ -20,8 +20,9 @@
     <sheet name="elements" sheetId="5" r:id="rId5"/>
     <sheet name="states" sheetId="6" r:id="rId6"/>
     <sheet name="parts" sheetId="9" r:id="rId7"/>
-    <sheet name="demand_models" sheetId="7" r:id="rId8"/>
-    <sheet name="demands" sheetId="8" r:id="rId9"/>
+    <sheet name="contents" sheetId="10" r:id="rId8"/>
+    <sheet name="demand_models" sheetId="7" r:id="rId9"/>
+    <sheet name="demands" sheetId="8" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="116">
   <si>
     <t>id</t>
   </si>
@@ -388,6 +389,9 @@
   </si>
   <si>
     <t>rate</t>
+  </si>
+  <si>
+    <t>container_id</t>
   </si>
 </sst>
 </file>
@@ -925,6 +929,44 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DA0B9F5-EAB2-45BD-9D78-117278B89EA3}">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7844D5C6-92A2-4B69-AF95-D74105C1704E}">
   <dimension ref="A1:J6"/>
@@ -1504,7 +1546,7 @@
   <dimension ref="A1:R14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2214,8 +2256,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C087CDB6-6E95-4070-A0DF-1ACAA4A5B0C0}">
   <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G72" sqref="G71:G72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2262,6 +2304,40 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABAF05E3-8DCE-4C51-83E2-9014172F15D6}">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F33A89FF-62A8-4D27-9DD4-AC6A11DA614F}">
   <dimension ref="A1:G1"/>
   <sheetViews>
@@ -2306,42 +2382,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DA0B9F5-EAB2-45BD-9D78-117278B89EA3}">
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D1" t="s">
-        <v>104</v>
-      </c>
-      <c r="E1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>